<commit_message>
Updated code, readme and command table
The code was developed with the help of team members
</commit_message>
<xml_diff>
--- a/command_table/Mesh_Project_Command_Table.xlsx
+++ b/command_table/Mesh_Project_Command_Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD1A724-D356-41DB-A801-274FA1124435}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059629D3-24DE-41BF-B132-B3F01F3C0AFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
-  <si>
-    <t>This node will implement the Client model (low power node which implements flame and gas sensor)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -82,9 +79,6 @@
     <t>factory reset timer handle, display update timer handle, log time timer handle, friend find timer handle</t>
   </si>
   <si>
-    <t>gecko_cmd_system_reset, displayUpdate, gecko_cmd_mesh_lpn_establish_friendship (only for LPN)</t>
-  </si>
-  <si>
     <t>gecko_evt_mesh_lpn_friendship_established_id, gecko_evt_mesh_lpn_friendship_failed_id (only for LPN)</t>
   </si>
   <si>
@@ -94,45 +88,12 @@
     <t>gecko_evt_mesh_node_initialized_id</t>
   </si>
   <si>
-    <t>provisioned &amp;&amp; DeviceUsesClientModel()</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_generic_client_init, lpn_init, gpioIntEnable</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Initialize the client model and does low power node initialization</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceUsesServerModel()</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_generic_server_init, gecko_cmd_mesh_friend_init()</t>
-  </si>
-  <si>
     <t>Initialize the server model and friend initialization</t>
   </si>
   <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,8)</t>
-  </si>
-  <si>
-    <t>Initialize the mesh library with support of up to 8 models</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffSubscriber()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,9), mesh_lib_generic_server_register_handler, mesh_lib_generic_server_update, mesh_lib_generic_server_publish</t>
-  </si>
-  <si>
-    <t>See init_models, onoff_request, onoff_update_and_publish in lightbulb.c, soc-btmesh-light example</t>
-  </si>
-  <si>
     <t>!provisioned</t>
   </si>
   <si>
@@ -166,9 +127,6 @@
     <t>gecko_evt_mesh_generic_server_client_request_id</t>
   </si>
   <si>
-    <t>DeviceUsesServerModel()</t>
-  </si>
-  <si>
     <t>mesh_lib_generic_server_event_handler</t>
   </si>
   <si>
@@ -199,24 +157,6 @@
     <t>Handle scheduler events</t>
   </si>
   <si>
-    <t>Button 0 press or release event &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
-    <t>mesh_lib_generic_client_publish</t>
-  </si>
-  <si>
-    <t>Publish button press or release using the on off model.  Press = on; will be updated for sensor</t>
-  </si>
-  <si>
-    <t>client request or server change callback for generic on/off model</t>
-  </si>
-  <si>
-    <t>Button Pressed or "Button Released"</t>
-  </si>
-  <si>
-    <t>Display the state of the button on the subscriber; will be updated for sensor</t>
-  </si>
-  <si>
     <t>On LPN side (used at this node)</t>
   </si>
   <si>
@@ -251,6 +191,24 @@
   </si>
   <si>
     <t>NOTE: This command table might be updated in future and code will be done accordingly. For now code is written such that it is capable of implementing both server and client functionality, however, the unrequired code will be removed in future.</t>
+  </si>
+  <si>
+    <t>This node will implement the Server model (low power node which implements flame and gas sensor)</t>
+  </si>
+  <si>
+    <t>mesh_lib_generic_server_publish</t>
+  </si>
+  <si>
+    <t>due to flame and gas sensor</t>
+  </si>
+  <si>
+    <t>gecko_cmd_mesh_generic_server_init, gecko_cmd_mesh_friend_init(), gpioIntEnable(), mesh_lib_init(malloc,free,9), mesh_lib_generic_server_register_handler</t>
+  </si>
+  <si>
+    <t>provisioned</t>
+  </si>
+  <si>
+    <t>gecko_cmd_system_reset, displayUpdate, gecko_cmd_mesh_lpn_establish_friendship</t>
   </si>
 </sst>
 </file>
@@ -577,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,405 +555,326 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
       </c>
       <c r="H20" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
-        <v>63</v>
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>76</v>
+      <c r="A25" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added persistent data and command table
</commit_message>
<xml_diff>
--- a/command_table/Mesh_Project_Command_Table.xlsx
+++ b/command_table/Mesh_Project_Command_Table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059629D3-24DE-41BF-B132-B3F01F3C0AFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E98192-C68F-4396-8971-41C996DA8BAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -49,9 +49,6 @@
     <t>gecko_evt_system_boot_id</t>
   </si>
   <si>
-    <t>button0 or button 1 pressed</t>
-  </si>
-  <si>
     <t>gecko_cmd_flash_ps_erase_all; gecko_cmd_hardware_set_soft_timer</t>
   </si>
   <si>
@@ -64,24 +61,12 @@
     <t>Factory reset and clear provisioner data for test purposes when either button is held on startup.  Must configure a timer to perform reset after 2 seconds</t>
   </si>
   <si>
-    <t>neither button0 or button 1 pressed</t>
-  </si>
-  <si>
-    <t>SetDeviceName; gecko_cmd_mesh_node_init</t>
-  </si>
-  <si>
     <t>gecko_evt_mesh_node_initialized</t>
   </si>
   <si>
     <t>Initialize the mesh stack</t>
   </si>
   <si>
-    <t>factory reset timer handle, display update timer handle, log time timer handle, friend find timer handle</t>
-  </si>
-  <si>
-    <t>gecko_evt_mesh_lpn_friendship_established_id, gecko_evt_mesh_lpn_friendship_failed_id (only for LPN)</t>
-  </si>
-  <si>
     <t>Completes factory reset, updates display for remove charge buildup, log timestamp value increase, tries to establish friendship on Client side</t>
   </si>
   <si>
@@ -91,9 +76,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Initialize the server model and friend initialization</t>
-  </si>
-  <si>
     <t>!provisioned</t>
   </si>
   <si>
@@ -154,18 +136,9 @@
     <t>gecko_evt_system_external_signal_id</t>
   </si>
   <si>
-    <t>Handle scheduler events</t>
-  </si>
-  <si>
-    <t>On LPN side (used at this node)</t>
-  </si>
-  <si>
     <t>gecko_evt_mesh_lpn_friendship_established_id</t>
   </si>
   <si>
-    <t>gecko_cmd_mesh_lpn_establish_friendship(0)</t>
-  </si>
-  <si>
     <t>LPN</t>
   </si>
   <si>
@@ -190,25 +163,52 @@
     <t>friend lost</t>
   </si>
   <si>
-    <t>NOTE: This command table might be updated in future and code will be done accordingly. For now code is written such that it is capable of implementing both server and client functionality, however, the unrequired code will be removed in future.</t>
-  </si>
-  <si>
-    <t>This node will implement the Server model (low power node which implements flame and gas sensor)</t>
-  </si>
-  <si>
-    <t>mesh_lib_generic_server_publish</t>
-  </si>
-  <si>
-    <t>due to flame and gas sensor</t>
-  </si>
-  <si>
     <t>gecko_cmd_mesh_generic_server_init, gecko_cmd_mesh_friend_init(), gpioIntEnable(), mesh_lib_init(malloc,free,9), mesh_lib_generic_server_register_handler</t>
   </si>
   <si>
     <t>provisioned</t>
   </si>
   <si>
-    <t>gecko_cmd_system_reset, displayUpdate, gecko_cmd_mesh_lpn_establish_friendship</t>
+    <t>Server Model (Low Power Node)</t>
+  </si>
+  <si>
+    <t>button 0 or button 1 pressed</t>
+  </si>
+  <si>
+    <t>neither button 0 or button 1 pressed</t>
+  </si>
+  <si>
+    <t>factory reset timer handle, display update timer handle, log time timer handle, friend find timer handle, alerts handle, interrupt drive sensor timeout events</t>
+  </si>
+  <si>
+    <t>gecko_cmd_system_reset, displayUpdate, gecko_cmd_mesh_lpn_establish_friendship, gecko_cmd_flash_ps_save</t>
+  </si>
+  <si>
+    <t>SetDeviceName; gecko_cmd_mesh_node_init; gecko_cmd_flash_ps_load</t>
+  </si>
+  <si>
+    <t>gecko_evt_mesh_lpn_friendship_established_id, gecko_evt_mesh_lpn_friendship_failed_id</t>
+  </si>
+  <si>
+    <t>Initialize the server model and friend initialization; also takes action based on saved persistent data</t>
+  </si>
+  <si>
+    <t>Deseralizes data when mesh generic request is received from friend</t>
+  </si>
+  <si>
+    <t>mesh_lib_generic_server_publish, gecko_cmd_flash_ps_save, gecko_cmd_hardware_set_soft_timer</t>
+  </si>
+  <si>
+    <t>Handle gas sensor scheduler events; fire sensor interrupt events; push button 0 interrupt and publishes required data; Also saves in persistent data</t>
+  </si>
+  <si>
+    <t>mesh_generic_request is received</t>
+  </si>
+  <si>
+    <t>gecko_cmd_mesh_lpn_establish_friendship</t>
+  </si>
+  <si>
+    <t>Flame sensor  interrupt and Gas sensor scheduler events and push button interrupt</t>
   </si>
 </sst>
 </file>
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,8 +554,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>57</v>
+      <c r="A1" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -589,19 +589,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -609,273 +609,275 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>58</v>
       </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
       <c r="H17" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
       <c r="H20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>